<commit_message>
ui done, cant submit
</commit_message>
<xml_diff>
--- a/dailycontest/data.xlsx
+++ b/dailycontest/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive\Desktop\iftikharul makatib\dailycontest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADC655E-B6D1-4109-9CDF-69644F26127B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F25B18-B786-4B96-AF50-825054BE1E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2DD21F5A-A335-4CF3-AA7A-5F21F5771062}"/>
   </bookViews>
@@ -404,10 +404,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}" name="Table1" displayName="Table1" ref="B2:D102" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}" name="Table1" displayName="Table1" ref="B2:D102" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="B2:D102" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C97">
     <sortCondition ref="C2:C97"/>
@@ -433,8 +433,8 @@
       <calculatedColumnFormula>IF(C3="","",ROW(A1))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{FC8865A0-2EB1-49B5-92A1-2871E0BB3F75}" name="name"/>
-    <tableColumn id="3" xr3:uid="{0EECEAAF-736A-4AE0-BB2F-1642CB7AF641}" name="html&lt;tag&gt;" dataDxfId="1">
-      <calculatedColumnFormula>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{0EECEAAF-736A-4AE0-BB2F-1642CB7AF641}" name="html&lt;tag&gt;" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -741,7 +741,7 @@
   <dimension ref="B2:G102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -776,8 +776,8 @@
         <v>75</v>
       </c>
       <c r="D3" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="1  احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)1&lt;"احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="1  احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)"&gt;1  احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)&lt;/option&gt;</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -789,8 +789,8 @@
         <v>38</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="2  اسمی بنت رفیع الدین  انصاری صاحب2&lt;"اسمی بنت رفیع الدین  انصاری صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="2  اسمی بنت رفیع الدین  انصاری صاحب"&gt;2  اسمی بنت رفیع الدین  انصاری صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -802,8 +802,8 @@
         <v>16</v>
       </c>
       <c r="D5" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="3  اشہر بن الطاف احمد صاحب3&lt;"اشہر بن الطاف احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="3  اشہر بن الطاف احمد صاحب"&gt;3  اشہر بن الطاف احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -815,8 +815,8 @@
         <v>30</v>
       </c>
       <c r="D6" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="4  آمنہ بنت حافظ انعام ا  لله صاحب4&lt;"آمنہ بنت حافظ انعام ا  لله صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="4  آمنہ بنت حافظ انعام ا  لله صاحب"&gt;4  آمنہ بنت حافظ انعام ا  لله صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -828,8 +828,8 @@
         <v>29</v>
       </c>
       <c r="D7" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="5  جویریہ بنت حافظ عصمت اللہ صاحب5&lt;"جویریہ بنت حافظ عصمت اللہ صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="5  جویریہ بنت حافظ عصمت اللہ صاحب"&gt;5  جویریہ بنت حافظ عصمت اللہ صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -841,8 +841,8 @@
         <v>76</v>
       </c>
       <c r="D8" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="6  خدیجہ  بنت دلشاد صاحب رح6&lt;"خدیجہ  بنت دلشاد صاحب رح&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="6  خدیجہ  بنت دلشاد صاحب رح"&gt;6  خدیجہ  بنت دلشاد صاحب رح&lt;/option&gt;</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
@@ -854,8 +854,8 @@
         <v>40</v>
       </c>
       <c r="D9" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="7  ذکری بنت جاوید حسین خان صاحب 7&lt;"ذکری بنت جاوید حسین خان صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="7  ذکری بنت جاوید حسین خان صاحب "&gt;7  ذکری بنت جاوید حسین خان صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -867,8 +867,8 @@
         <v>77</v>
       </c>
       <c r="D10" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="8  رضا بنت نوشاد صاحب8&lt;"رضا بنت نوشاد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="8  رضا بنت نوشاد صاحب"&gt;8  رضا بنت نوشاد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -880,8 +880,8 @@
         <v>100</v>
       </c>
       <c r="D11" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="9  زینب بنت بدرالزماں صاحب9&lt;"زینب بنت بدرالزماں صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="9  زینب بنت بدرالزماں صاحب"&gt;9  زینب بنت بدرالزماں صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -893,8 +893,8 @@
         <v>51</v>
       </c>
       <c r="D12" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="10  زینت خاتون بنت عبد الحسن صاحب10&lt;"زینت خاتون بنت عبد الحسن صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="10  زینت خاتون بنت عبد الحسن صاحب"&gt;10  زینت خاتون بنت عبد الحسن صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -906,8 +906,8 @@
         <v>79</v>
       </c>
       <c r="D13" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="11  شیزان رحمت بن رحمت علی صاحب (بستی)11&lt;"شیزان رحمت بن رحمت علی صاحب (بستی)&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="11  شیزان رحمت بن رحمت علی صاحب (بستی)"&gt;11  شیزان رحمت بن رحمت علی صاحب (بستی)&lt;/option&gt;</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -919,8 +919,8 @@
         <v>78</v>
       </c>
       <c r="D14" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="12  صفوان بن رحمت علی  صاحب (بستی)12&lt;"صفوان بن رحمت علی  صاحب (بستی)&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="12  صفوان بن رحمت علی  صاحب (بستی)"&gt;12  صفوان بن رحمت علی  صاحب (بستی)&lt;/option&gt;</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -932,8 +932,8 @@
         <v>37</v>
       </c>
       <c r="D15" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="13  عائشہ بنت  محمّد معشوق صاحب13&lt;"عائشہ بنت  محمّد معشوق صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="13  عائشہ بنت  محمّد معشوق صاحب"&gt;13  عائشہ بنت  محمّد معشوق صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
@@ -945,8 +945,8 @@
         <v>43</v>
       </c>
       <c r="D16" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="14  عبدالصمد  بن محمّد شفیع صاحب14&lt;"عبدالصمد  بن محمّد شفیع صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="14  عبدالصمد  بن محمّد شفیع صاحب"&gt;14  عبدالصمد  بن محمّد شفیع صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -958,8 +958,8 @@
         <v>80</v>
       </c>
       <c r="D17" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="15  علیشا بنت دلشاد صاحب رح15&lt;"علیشا بنت دلشاد صاحب رح&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="15  علیشا بنت دلشاد صاحب رح"&gt;15  علیشا بنت دلشاد صاحب رح&lt;/option&gt;</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
@@ -971,8 +971,8 @@
         <v>48</v>
       </c>
       <c r="D18" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="16  عیاض احمد بن فرحت حسین صاحب16&lt;"عیاض احمد بن فرحت حسین صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="16  عیاض احمد بن فرحت حسین صاحب"&gt;16  عیاض احمد بن فرحت حسین صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
@@ -984,8 +984,8 @@
         <v>7</v>
       </c>
       <c r="D19" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="17  عیاض احمد بن وسیم احمد صاحب17&lt;"عیاض احمد بن وسیم احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="17  عیاض احمد بن وسیم احمد صاحب"&gt;17  عیاض احمد بن وسیم احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
@@ -997,8 +997,8 @@
         <v>81</v>
       </c>
       <c r="D20" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="18  فضا بنت قاری صفی اللہ  صاحب18&lt;"فضا بنت قاری صفی اللہ  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="18  فضا بنت قاری صفی اللہ  صاحب"&gt;18  فضا بنت قاری صفی اللہ  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
@@ -1010,8 +1010,8 @@
         <v>82</v>
       </c>
       <c r="D21" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="19  فہد صادق بن عبد الصادق صاحب رح19&lt;"فہد صادق بن عبد الصادق صاحب رح&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="19  فہد صادق بن عبد الصادق صاحب رح"&gt;19  فہد صادق بن عبد الصادق صاحب رح&lt;/option&gt;</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.3">
@@ -1023,8 +1023,8 @@
         <v>69</v>
       </c>
       <c r="D22" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="20  محمّد  فہد  بن غیاث صاحب20&lt;"محمّد  فہد  بن غیاث صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="20  محمّد  فہد  بن غیاث صاحب"&gt;20  محمّد  فہد  بن غیاث صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.3">
@@ -1036,8 +1036,8 @@
         <v>71</v>
       </c>
       <c r="D23" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="21  محمّد  مصطفیٰ بن فرمان حشمت صاحب21&lt;"محمّد  مصطفیٰ بن فرمان حشمت صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="21  محمّد  مصطفیٰ بن فرمان حشمت صاحب"&gt;21  محمّد  مصطفیٰ بن فرمان حشمت صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.3">
@@ -1049,8 +1049,8 @@
         <v>41</v>
       </c>
       <c r="D24" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="22  محمّد ابان بن محمّد عامر صاحب22&lt;"محمّد ابان بن محمّد عامر صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="22  محمّد ابان بن محمّد عامر صاحب"&gt;22  محمّد ابان بن محمّد عامر صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
@@ -1062,8 +1062,8 @@
         <v>23</v>
       </c>
       <c r="D25" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="23  محمّد ابراہیم بن محمّد ارشاد  صاحب23&lt;"محمّد ابراہیم بن محمّد ارشاد  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="23  محمّد ابراہیم بن محمّد ارشاد  صاحب"&gt;23  محمّد ابراہیم بن محمّد ارشاد  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.3">
@@ -1075,8 +1075,8 @@
         <v>83</v>
       </c>
       <c r="D26" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="24  محمّد احتشام بن قاری صفی الله صاحب24&lt;"محمّد احتشام بن قاری صفی الله صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="24  محمّد احتشام بن قاری صفی الله صاحب"&gt;24  محمّد احتشام بن قاری صفی الله صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.3">
@@ -1088,8 +1088,8 @@
         <v>84</v>
       </c>
       <c r="D27" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="25  محمّد اذلان بن علیم عارف صاحب25&lt;"محمّد اذلان بن علیم عارف صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="25  محمّد اذلان بن علیم عارف صاحب"&gt;25  محمّد اذلان بن علیم عارف صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
@@ -1101,8 +1101,8 @@
         <v>19</v>
       </c>
       <c r="D28" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="26  محمّد اذہان بن پرویز احمد صاحب26&lt;"محمّد اذہان بن پرویز احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="26  محمّد اذہان بن پرویز احمد صاحب"&gt;26  محمّد اذہان بن پرویز احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.3">
@@ -1114,8 +1114,8 @@
         <v>85</v>
       </c>
       <c r="D29" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="27  محمّد ارحان بن محمّد اختر صاحب27&lt;"محمّد ارحان بن محمّد اختر صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="27  محمّد ارحان بن محمّد اختر صاحب"&gt;27  محمّد ارحان بن محمّد اختر صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">
@@ -1127,8 +1127,8 @@
         <v>18</v>
       </c>
       <c r="D30" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="28  محمّد ارحم بن   قمر الہدی صاحب28&lt;"محمّد ارحم بن   قمر الہدی صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="28  محمّد ارحم بن   قمر الہدی صاحب"&gt;28  محمّد ارحم بن   قمر الہدی صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.3">
@@ -1140,8 +1140,8 @@
         <v>39</v>
       </c>
       <c r="D31" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="29  محمّد ارسلان بن محمّد افضل صاحب29&lt;"محمّد ارسلان بن محمّد افضل صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="29  محمّد ارسلان بن محمّد افضل صاحب"&gt;29  محمّد ارسلان بن محمّد افضل صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.3">
@@ -1153,8 +1153,8 @@
         <v>4</v>
       </c>
       <c r="D32" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="30  محمّد ارکان بن محمّد محفوظ صاحب30&lt;"محمّد ارکان بن محمّد محفوظ صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="30  محمّد ارکان بن محمّد محفوظ صاحب"&gt;30  محمّد ارکان بن محمّد محفوظ صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.3">
@@ -1166,8 +1166,8 @@
         <v>87</v>
       </c>
       <c r="D33" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="31  محمّد الحم بن افروز اختر صاحب31&lt;"محمّد الحم بن افروز اختر صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="31  محمّد الحم بن افروز اختر صاحب"&gt;31  محمّد الحم بن افروز اختر صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.3">
@@ -1179,8 +1179,8 @@
         <v>13</v>
       </c>
       <c r="D34" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="32  محمّد امان بن الطاف احمد صاحب32&lt;"محمّد امان بن الطاف احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="32  محمّد امان بن الطاف احمد صاحب"&gt;32  محمّد امان بن الطاف احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.3">
@@ -1192,8 +1192,8 @@
         <v>86</v>
       </c>
       <c r="D35" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="33  محمّد امان بن بدر الزماں صاحب 33&lt;"محمّد امان بن بدر الزماں صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="33  محمّد امان بن بدر الزماں صاحب "&gt;33  محمّد امان بن بدر الزماں صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.3">
@@ -1205,8 +1205,8 @@
         <v>88</v>
       </c>
       <c r="D36" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="34  محمّد امان بن راشد الحق صاحب34&lt;"محمّد امان بن راشد الحق صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="34  محمّد امان بن راشد الحق صاحب"&gt;34  محمّد امان بن راشد الحق صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.3">
@@ -1218,8 +1218,8 @@
         <v>1</v>
       </c>
       <c r="D37" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="35  محمّد انس بن   محمّد چاند صاحب35&lt;"محمّد انس بن   محمّد چاند صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="35  محمّد انس بن   محمّد چاند صاحب"&gt;35  محمّد انس بن   محمّد چاند صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.3">
@@ -1231,8 +1231,8 @@
         <v>89</v>
       </c>
       <c r="D38" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="36  محمّد ایذان بن محمّد عالم صاحب36&lt;"محمّد ایذان بن محمّد عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="36  محمّد ایذان بن محمّد عالم صاحب"&gt;36  محمّد ایذان بن محمّد عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.3">
@@ -1244,8 +1244,8 @@
         <v>53</v>
       </c>
       <c r="D39" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="37  محمّد آشد  بن غیاث  صاحب37&lt;"محمّد آشد  بن غیاث  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="37  محمّد آشد  بن غیاث  صاحب"&gt;37  محمّد آشد  بن غیاث  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.3">
@@ -1257,8 +1257,8 @@
         <v>55</v>
       </c>
       <c r="D40" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="38  محمّد آفرید بن وسیم احمد صاحب 38&lt;"محمّد آفرید بن وسیم احمد صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="38  محمّد آفرید بن وسیم احمد صاحب "&gt;38  محمّد آفرید بن وسیم احمد صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.3">
@@ -1270,8 +1270,8 @@
         <v>15</v>
       </c>
       <c r="D41" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="39  محمّد بلال بن انور حسین صاحب39&lt;"محمّد بلال بن انور حسین صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="39  محمّد بلال بن انور حسین صاحب"&gt;39  محمّد بلال بن انور حسین صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.3">
@@ -1283,8 +1283,8 @@
         <v>27</v>
       </c>
       <c r="D42" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="40  محمّد تنزیل  بن حسن مطلوب صاحب40&lt;"محمّد تنزیل  بن حسن مطلوب صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="40  محمّد تنزیل  بن حسن مطلوب صاحب"&gt;40  محمّد تنزیل  بن حسن مطلوب صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.3">
@@ -1296,8 +1296,8 @@
         <v>62</v>
       </c>
       <c r="D43" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="41  محمّد تہشیم   بن  ندیم  احمد صاحب41&lt;"محمّد تہشیم   بن  ندیم  احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="41  محمّد تہشیم   بن  ندیم  احمد صاحب"&gt;41  محمّد تہشیم   بن  ندیم  احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.3">
@@ -1309,8 +1309,8 @@
         <v>26</v>
       </c>
       <c r="D44" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="42  محمّد توحیدبن حسن مطلوب صاحب42&lt;"محمّد توحیدبن حسن مطلوب صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="42  محمّد توحیدبن حسن مطلوب صاحب"&gt;42  محمّد توحیدبن حسن مطلوب صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.3">
@@ -1322,8 +1322,8 @@
         <v>14</v>
       </c>
       <c r="D45" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="43  محمّد حمّاد بن عدیل  احمد  صاحب43&lt;"محمّد حمّاد بن عدیل  احمد  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="43  محمّد حمّاد بن عدیل  احمد  صاحب"&gt;43  محمّد حمّاد بن عدیل  احمد  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.3">
@@ -1335,8 +1335,8 @@
         <v>6</v>
       </c>
       <c r="D46" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="44  محمّد حمزہ   اسرائیل صاحب44&lt;"محمّد حمزہ   اسرائیل صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="44  محمّد حمزہ   اسرائیل صاحب"&gt;44  محمّد حمزہ   اسرائیل صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.3">
@@ -1348,8 +1348,8 @@
         <v>36</v>
       </c>
       <c r="D47" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="45  محمّد حمزہ  بن غلام رسول صاحب 45&lt;"محمّد حمزہ  بن غلام رسول صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="45  محمّد حمزہ  بن غلام رسول صاحب "&gt;45  محمّد حمزہ  بن غلام رسول صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.3">
@@ -1361,8 +1361,8 @@
         <v>10</v>
       </c>
       <c r="D48" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="46  محمّد حمزہ بن مہتاب عالم صاحب46&lt;"محمّد حمزہ بن مہتاب عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="46  محمّد حمزہ بن مہتاب عالم صاحب"&gt;46  محمّد حمزہ بن مہتاب عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.3">
@@ -1374,8 +1374,8 @@
         <v>9</v>
       </c>
       <c r="D49" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="47  محمّد حمید بن شاداب عالم صاحب47&lt;"محمّد حمید بن شاداب عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="47  محمّد حمید بن شاداب عالم صاحب"&gt;47  محمّد حمید بن شاداب عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.3">
@@ -1387,8 +1387,8 @@
         <v>0</v>
       </c>
       <c r="D50" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="48  محمّد حنیف بن ملک الافضل صاحب 48&lt;"محمّد حنیف بن ملک الافضل صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="48  محمّد حنیف بن ملک الافضل صاحب "&gt;48  محمّد حنیف بن ملک الافضل صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.3">
@@ -1400,8 +1400,8 @@
         <v>8</v>
       </c>
       <c r="D51" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="49  محمّد دارین بن محمّد عامر صاحب49&lt;"محمّد دارین بن محمّد عامر صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="49  محمّد دارین بن محمّد عامر صاحب"&gt;49  محمّد دارین بن محمّد عامر صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.3">
@@ -1413,8 +1413,8 @@
         <v>90</v>
       </c>
       <c r="D52" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="50  محمّد دانش بن نصیر احمد صاحب50&lt;"محمّد دانش بن نصیر احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="50  محمّد دانش بن نصیر احمد صاحب"&gt;50  محمّد دانش بن نصیر احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.3">
@@ -1426,8 +1426,8 @@
         <v>52</v>
       </c>
       <c r="D53" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="51  محمّد داؤد بن خواجہ فرید الدین  صاحب51&lt;"محمّد داؤد بن خواجہ فرید الدین  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="51  محمّد داؤد بن خواجہ فرید الدین  صاحب"&gt;51  محمّد داؤد بن خواجہ فرید الدین  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.3">
@@ -1439,8 +1439,8 @@
         <v>35</v>
       </c>
       <c r="D54" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="52  محمّد راشد بن رازق حسین خان صاحب52&lt;"محمّد راشد بن رازق حسین خان صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="52  محمّد راشد بن رازق حسین خان صاحب"&gt;52  محمّد راشد بن رازق حسین خان صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.3">
@@ -1452,8 +1452,8 @@
         <v>22</v>
       </c>
       <c r="D55" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="53  محمّد ریحان  بن شمیم عالم صاحب53&lt;"محمّد ریحان  بن شمیم عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="53  محمّد ریحان  بن شمیم عالم صاحب"&gt;53  محمّد ریحان  بن شمیم عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.3">
@@ -1465,8 +1465,8 @@
         <v>54</v>
       </c>
       <c r="D56" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="54  محمّد ریحان بن اظہار احمد صاحب54&lt;"محمّد ریحان بن اظہار احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="54  محمّد ریحان بن اظہار احمد صاحب"&gt;54  محمّد ریحان بن اظہار احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.3">
@@ -1478,8 +1478,8 @@
         <v>47</v>
       </c>
       <c r="D57" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="55  محمّد زیان بن رضوان خان صاحب55&lt;"محمّد زیان بن رضوان خان صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="55  محمّد زیان بن رضوان خان صاحب"&gt;55  محمّد زیان بن رضوان خان صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.3">
@@ -1491,8 +1491,8 @@
         <v>70</v>
       </c>
       <c r="D58" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="56  محمّد زید بن  افتخار  احمد  صاحب56&lt;"محمّد زید بن  افتخار  احمد  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="56  محمّد زید بن  افتخار  احمد  صاحب"&gt;56  محمّد زید بن  افتخار  احمد  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.3">
@@ -1504,8 +1504,8 @@
         <v>57</v>
       </c>
       <c r="D59" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="57  محمّد زید بن حافظ فیض الرحمن صاحب57&lt;"محمّد زید بن حافظ فیض الرحمن صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="57  محمّد زید بن حافظ فیض الرحمن صاحب"&gt;57  محمّد زید بن حافظ فیض الرحمن صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.3">
@@ -1517,8 +1517,8 @@
         <v>61</v>
       </c>
       <c r="D60" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="58  محمّد زید بن ظہیر الدین صاحب58&lt;"محمّد زید بن ظہیر الدین صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="58  محمّد زید بن ظہیر الدین صاحب"&gt;58  محمّد زید بن ظہیر الدین صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.3">
@@ -1530,8 +1530,8 @@
         <v>44</v>
       </c>
       <c r="D61" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="59  محمّد سفیان بن شفقت الله صاحب59&lt;"محمّد سفیان بن شفقت الله صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="59  محمّد سفیان بن شفقت الله صاحب"&gt;59  محمّد سفیان بن شفقت الله صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.3">
@@ -1543,8 +1543,8 @@
         <v>20</v>
       </c>
       <c r="D62" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="60  محمّد شادمان  بن محمّد ارشاد صاحب60&lt;"محمّد شادمان  بن محمّد ارشاد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="60  محمّد شادمان  بن محمّد ارشاد صاحب"&gt;60  محمّد شادمان  بن محمّد ارشاد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.3">
@@ -1556,8 +1556,8 @@
         <v>5</v>
       </c>
       <c r="D63" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="61  محمّد شمس بن پرویز لاری صاحب61&lt;"محمّد شمس بن پرویز لاری صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="61  محمّد شمس بن پرویز لاری صاحب"&gt;61  محمّد شمس بن پرویز لاری صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.3">
@@ -1569,8 +1569,8 @@
         <v>46</v>
       </c>
       <c r="D64" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="62  محمّد صالق بن واثق باللہ صاحب62&lt;"محمّد صالق بن واثق باللہ صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="62  محمّد صالق بن واثق باللہ صاحب"&gt;62  محمّد صالق بن واثق باللہ صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.3">
@@ -1582,8 +1582,8 @@
         <v>91</v>
       </c>
       <c r="D65" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="63  محمّد صائم بن محمّد فیصل صاحب63&lt;"محمّد صائم بن محمّد فیصل صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="63  محمّد صائم بن محمّد فیصل صاحب"&gt;63  محمّد صائم بن محمّد فیصل صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.3">
@@ -1595,8 +1595,8 @@
         <v>17</v>
       </c>
       <c r="D66" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="64  محمّد صفوان بن محمّد قیصر عالم صاحب64&lt;"محمّد صفوان بن محمّد قیصر عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="64  محمّد صفوان بن محمّد قیصر عالم صاحب"&gt;64  محمّد صفوان بن محمّد قیصر عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.3">
@@ -1608,8 +1608,8 @@
         <v>64</v>
       </c>
       <c r="D67" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="65  محمّد طیّب  بن مہتاب عالم صاحب65&lt;"محمّد طیّب  بن مہتاب عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="65  محمّد طیّب  بن مہتاب عالم صاحب"&gt;65  محمّد طیّب  بن مہتاب عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.3">
@@ -1621,8 +1621,8 @@
         <v>56</v>
       </c>
       <c r="D68" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="66  محمّد عابدبن حافظ عمران صاحب66&lt;"محمّد عابدبن حافظ عمران صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="66  محمّد عابدبن حافظ عمران صاحب"&gt;66  محمّد عابدبن حافظ عمران صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.3">
@@ -1634,8 +1634,8 @@
         <v>92</v>
       </c>
       <c r="D69" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="67  محمّد عارش  بن علیم الدین صاحب67&lt;"محمّد عارش  بن علیم الدین صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="67  محمّد عارش  بن علیم الدین صاحب"&gt;67  محمّد عارش  بن علیم الدین صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.3">
@@ -1647,8 +1647,8 @@
         <v>31</v>
       </c>
       <c r="D70" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="68  محمّد عاکف بن قمرالہدی صاحب68&lt;"محمّد عاکف بن قمرالہدی صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="68  محمّد عاکف بن قمرالہدی صاحب"&gt;68  محمّد عاکف بن قمرالہدی صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.3">
@@ -1660,8 +1660,8 @@
         <v>45</v>
       </c>
       <c r="D71" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="69  محمّد عاہل بن محمّد دانش  صاحب69&lt;"محمّد عاہل بن محمّد دانش  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="69  محمّد عاہل بن محمّد دانش  صاحب"&gt;69  محمّد عاہل بن محمّد دانش  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.3">
@@ -1673,8 +1673,8 @@
         <v>33</v>
       </c>
       <c r="D72" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="70  محمّد عدنان بن محمّد افضل صاحب70&lt;"محمّد عدنان بن محمّد افضل صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="70  محمّد عدنان بن محمّد افضل صاحب"&gt;70  محمّد عدنان بن محمّد افضل صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.3">
@@ -1686,8 +1686,8 @@
         <v>63</v>
       </c>
       <c r="D73" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="71  محمّد عزیر بن ممتاز احمد صاحب71&lt;"محمّد عزیر بن ممتاز احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="71  محمّد عزیر بن ممتاز احمد صاحب"&gt;71  محمّد عزیر بن ممتاز احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.3">
@@ -1699,8 +1699,8 @@
         <v>93</v>
       </c>
       <c r="D74" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="72  محمّد علی بن نوید احمد صاحب72&lt;"محمّد علی بن نوید احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="72  محمّد علی بن نوید احمد صاحب"&gt;72  محمّد علی بن نوید احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.3">
@@ -1712,8 +1712,8 @@
         <v>3</v>
       </c>
       <c r="D75" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="73  محمّد عمر بن عبد الرزاق صاحب73&lt;"محمّد عمر بن عبد الرزاق صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="73  محمّد عمر بن عبد الرزاق صاحب"&gt;73  محمّد عمر بن عبد الرزاق صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
@@ -1725,8 +1725,8 @@
         <v>34</v>
       </c>
       <c r="D76" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="74  محمّد عمر بن گلریز احمد خان صاحب74&lt;"محمّد عمر بن گلریز احمد خان صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="74  محمّد عمر بن گلریز احمد خان صاحب"&gt;74  محمّد عمر بن گلریز احمد خان صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.3">
@@ -1738,8 +1738,8 @@
         <v>67</v>
       </c>
       <c r="D77" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="75  محمّد عمیر بن نذیر الدین صاحب75&lt;"محمّد عمیر بن نذیر الدین صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="75  محمّد عمیر بن نذیر الدین صاحب"&gt;75  محمّد عمیر بن نذیر الدین صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
@@ -1751,8 +1751,8 @@
         <v>72</v>
       </c>
       <c r="D78" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="76  محمّد عیاں بن شفیق صاحب رحمه اللہ76&lt;"محمّد عیاں بن شفیق صاحب رحمه اللہ&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="76  محمّد عیاں بن شفیق صاحب رحمه اللہ"&gt;76  محمّد عیاں بن شفیق صاحب رحمه اللہ&lt;/option&gt;</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.3">
@@ -1764,8 +1764,8 @@
         <v>94</v>
       </c>
       <c r="D79" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="77  محمّد عیان بن ظہیر الدین صاحب77&lt;"محمّد عیان بن ظہیر الدین صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="77  محمّد عیان بن ظہیر الدین صاحب"&gt;77  محمّد عیان بن ظہیر الدین صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.3">
@@ -1777,8 +1777,8 @@
         <v>58</v>
       </c>
       <c r="D80" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="78  محمّد فرحان بن شمیم عالم صاحب78&lt;"محمّد فرحان بن شمیم عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="78  محمّد فرحان بن شمیم عالم صاحب"&gt;78  محمّد فرحان بن شمیم عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.3">
@@ -1790,8 +1790,8 @@
         <v>21</v>
       </c>
       <c r="D81" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="79  محمّد فردین بن محمّد شاہد صاحب79&lt;"محمّد فردین بن محمّد شاہد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="79  محمّد فردین بن محمّد شاہد صاحب"&gt;79  محمّد فردین بن محمّد شاہد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
@@ -1803,8 +1803,8 @@
         <v>11</v>
       </c>
       <c r="D82" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="80  محمّد کیفی بن محمّد نواز شیروانی صاحب80&lt;"محمّد کیفی بن محمّد نواز شیروانی صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="80  محمّد کیفی بن محمّد نواز شیروانی صاحب"&gt;80  محمّد کیفی بن محمّد نواز شیروانی صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.3">
@@ -1816,8 +1816,8 @@
         <v>32</v>
       </c>
       <c r="D83" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="81  محمّد محتشم بن محمّد عامر صاحب81&lt;"محمّد محتشم بن محمّد عامر صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="81  محمّد محتشم بن محمّد عامر صاحب"&gt;81  محمّد محتشم بن محمّد عامر صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.3">
@@ -1829,8 +1829,8 @@
         <v>59</v>
       </c>
       <c r="D84" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="82  محمّد مدّثر بن شکیل احمد  صاحب82&lt;"محمّد مدّثر بن شکیل احمد  صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="82  محمّد مدّثر بن شکیل احمد  صاحب"&gt;82  محمّد مدّثر بن شکیل احمد  صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
@@ -1842,8 +1842,8 @@
         <v>49</v>
       </c>
       <c r="D85" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="83  محمّد مزمل بن شکیل احمد صاحب83&lt;"محمّد مزمل بن شکیل احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="83  محمّد مزمل بن شکیل احمد صاحب"&gt;83  محمّد مزمل بن شکیل احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
@@ -1855,8 +1855,8 @@
         <v>60</v>
       </c>
       <c r="D86" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="84  محمّد معروف بن  محمّد معشوق صاحب84&lt;"محمّد معروف بن  محمّد معشوق صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="84  محمّد معروف بن  محمّد معشوق صاحب"&gt;84  محمّد معروف بن  محمّد معشوق صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.3">
@@ -1868,8 +1868,8 @@
         <v>25</v>
       </c>
       <c r="D87" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="85  محمّد ہادی بن ملک العزیز صاحب85&lt;"محمّد ہادی بن ملک العزیز صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="85  محمّد ہادی بن ملک العزیز صاحب"&gt;85  محمّد ہادی بن ملک العزیز صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.3">
@@ -1881,8 +1881,8 @@
         <v>2</v>
       </c>
       <c r="D88" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="86  محمّد ھود 86&lt;"محمّد ھود &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="86  محمّد ھود "&gt;86  محمّد ھود &lt;/option&gt;</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.3">
@@ -1894,8 +1894,8 @@
         <v>68</v>
       </c>
       <c r="D89" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="87  محمّد یوسف بن ذرار صاحب87&lt;"محمّد یوسف بن ذرار صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="87  محمّد یوسف بن ذرار صاحب"&gt;87  محمّد یوسف بن ذرار صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.3">
@@ -1907,8 +1907,8 @@
         <v>50</v>
       </c>
       <c r="D90" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="88  محمّد یوسف بن محمّد بلال صاحب 88&lt;"محمّد یوسف بن محمّد بلال صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="88  محمّد یوسف بن محمّد بلال صاحب "&gt;88  محمّد یوسف بن محمّد بلال صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.3">
@@ -1920,8 +1920,8 @@
         <v>95</v>
       </c>
       <c r="D91" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="89  محمّداحتشام بن نعیم خان صاحب89&lt;"محمّداحتشام بن نعیم خان صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="89  محمّداحتشام بن نعیم خان صاحب"&gt;89  محمّداحتشام بن نعیم خان صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.3">
@@ -1933,8 +1933,8 @@
         <v>24</v>
       </c>
       <c r="D92" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="90  محمّدشدیب  بن محمّد عالم صاحب90&lt;"محمّدشدیب  بن محمّد عالم صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="90  محمّدشدیب  بن محمّد عالم صاحب"&gt;90  محمّدشدیب  بن محمّد عالم صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.3">
@@ -1946,8 +1946,8 @@
         <v>42</v>
       </c>
       <c r="D93" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="91  محمّدعرش  بن عبد الرحیم صاحب 91&lt;"محمّدعرش  بن عبد الرحیم صاحب &lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="91  محمّدعرش  بن عبد الرحیم صاحب "&gt;91  محمّدعرش  بن عبد الرحیم صاحب &lt;/option&gt;</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.3">
@@ -1959,8 +1959,8 @@
         <v>66</v>
       </c>
       <c r="D94" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="92  معاذ حبیب بن حبیب الله صاحب92&lt;"معاذ حبیب بن حبیب الله صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="92  معاذ حبیب بن حبیب الله صاحب"&gt;92  معاذ حبیب بن حبیب الله صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.3">
@@ -1972,8 +1972,8 @@
         <v>28</v>
       </c>
       <c r="D95" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="93  معاذ رحمن بن معین الرحمن صاحب93&lt;"معاذ رحمن بن معین الرحمن صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="93  معاذ رحمن بن معین الرحمن صاحب"&gt;93  معاذ رحمن بن معین الرحمن صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.3">
@@ -1985,8 +1985,8 @@
         <v>12</v>
       </c>
       <c r="D96" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="94  وصی احمد بن رئیس احمد صاحب94&lt;"وصی احمد بن رئیس احمد صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="94  وصی احمد بن رئیس احمد صاحب"&gt;94  وصی احمد بن رئیس احمد صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.3">
@@ -1998,8 +1998,8 @@
         <v>65</v>
       </c>
       <c r="D97" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="95  یٰسین کاظمی بن قطب الدین  کاظمی صاحب95&lt;"یٰسین کاظمی بن قطب الدین  کاظمی صاحب&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="95  یٰسین کاظمی بن قطب الدین  کاظمی صاحب"&gt;95  یٰسین کاظمی بن قطب الدین  کاظمی صاحب&lt;/option&gt;</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.3">
@@ -2011,8 +2011,8 @@
         <v>96</v>
       </c>
       <c r="D98" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="96  محمّد طالب بن96&lt;"محمّد طالب بن&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="96  محمّد طالب بن"&gt;96  محمّد طالب بن&lt;/option&gt;</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.3">
@@ -2024,8 +2024,8 @@
         <v>97</v>
       </c>
       <c r="D99" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="97  محمّد ذہیب بن97&lt;"محمّد ذہیب بن&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="97  محمّد ذہیب بن"&gt;97  محمّد ذہیب بن&lt;/option&gt;</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.3">
@@ -2037,8 +2037,8 @@
         <v>104</v>
       </c>
       <c r="D100" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="98  محمّد عمر بن محمّد اجمل صاحب  (مئو)98&lt;"محمّد عمر بن محمّد اجمل صاحب  (مئو)&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="98  محمّد عمر بن محمّد اجمل صاحب  (مئو)"&gt;98  محمّد عمر بن محمّد اجمل صاحب  (مئو)&lt;/option&gt;</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.3">
@@ -2050,8 +2050,8 @@
         <v>98</v>
       </c>
       <c r="D101" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="99  محمّد زیاں بن محمّد انور صاحب (امریکا)99&lt;"محمّد زیاں بن محمّد انور صاحب (امریکا)&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="99  محمّد زیاں بن محمّد انور صاحب (امریکا)"&gt;99  محمّد زیاں بن محمّد انور صاحب (امریکا)&lt;/option&gt;</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.3">
@@ -2063,8 +2063,8 @@
         <v>99</v>
       </c>
       <c r="D102" t="str">
-        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],Table1[[#This Row],[roll-no]],"&lt;""",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
-        <v>&lt;option value="100  محمّد ریاض صاحب (جدّہ)100&lt;"محمّد ریاض صاحب (جدّہ)&lt;/option&gt;</v>
+        <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
+        <v>&lt;option value="100  محمّد ریاض صاحب (جدّہ)"&gt;100  محمّد ریاض صاحب (جدّہ)&lt;/option&gt;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
name + no. col added
</commit_message>
<xml_diff>
--- a/dailycontest/data.xlsx
+++ b/dailycontest/data.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\OneDrive\Desktop\iftikharul makatib\dailycontest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F25B18-B786-4B96-AF50-825054BE1E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1878A9C7-17ED-404C-ABC4-56AD4A1ADE3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2DD21F5A-A335-4CF3-AA7A-5F21F5771062}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="name">Table1[rollno+name]</definedName>
+    <definedName name="names">Table1[rollno+name]</definedName>
+    <definedName name="options">Table1[rollno+name]</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="106">
   <si>
     <t xml:space="preserve">محمّد حنیف بن ملک الافضل صاحب </t>
   </si>
@@ -350,6 +355,9 @@
   </si>
   <si>
     <t>محمّد عمر بن محمّد اجمل صاحب  (مئو)</t>
+  </si>
+  <si>
+    <t>rollno+name</t>
   </si>
 </sst>
 </file>
@@ -402,7 +410,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -423,18 +434,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}" name="Table1" displayName="Table1" ref="B2:D102" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="B2:D102" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}" name="Table1" displayName="Table1" ref="B2:E102" totalsRowShown="0" headerRowDxfId="2">
+  <autoFilter ref="B2:E102" xr:uid="{0720B3ED-E398-46AF-B2A4-A7DE79BC1F81}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:C97">
     <sortCondition ref="C2:C97"/>
   </sortState>
-  <tableColumns count="3">
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{112DB414-D5F1-4ACE-B837-9762DC3CAF4F}" name="roll-no">
       <calculatedColumnFormula>IF(C3="","",ROW(A1))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{FC8865A0-2EB1-49B5-92A1-2871E0BB3F75}" name="name"/>
-    <tableColumn id="3" xr3:uid="{0EECEAAF-736A-4AE0-BB2F-1642CB7AF641}" name="html&lt;tag&gt;" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{0EECEAAF-736A-4AE0-BB2F-1642CB7AF641}" name="html&lt;tag&gt;" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{49854B69-60EA-4814-BECA-6F756282E744}" name="rollno+name" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -738,19 +752,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A23E516-3FF1-478F-A7A5-0753CE97A22D}">
-  <dimension ref="B2:G102"/>
+  <dimension ref="B2:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="43.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="99.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>73</v>
       </c>
@@ -760,14 +775,17 @@
       <c r="D2" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J2" t="s">
         <v>102</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B3">
         <f t="shared" ref="B3:B66" si="0">IF(C3="","",ROW(A1))</f>
         <v>1</v>
@@ -779,8 +797,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="1  احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)"&gt;1  احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E3" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>1    احمد حسن بن  ابرار احمد انصاری  صاحب (جھانسی)</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B4">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -792,8 +814,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="2  اسمی بنت رفیع الدین  انصاری صاحب"&gt;2  اسمی بنت رفیع الدین  انصاری صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E4" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>2    اسمی بنت رفیع الدین  انصاری صاحب</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B5">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -805,8 +831,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="3  اشہر بن الطاف احمد صاحب"&gt;3  اشہر بن الطاف احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E5" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>3    اشہر بن الطاف احمد صاحب</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -818,8 +848,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="4  آمنہ بنت حافظ انعام ا  لله صاحب"&gt;4  آمنہ بنت حافظ انعام ا  لله صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E6" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>4    آمنہ بنت حافظ انعام ا  لله صاحب</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -831,8 +865,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="5  جویریہ بنت حافظ عصمت اللہ صاحب"&gt;5  جویریہ بنت حافظ عصمت اللہ صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E7" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>5    جویریہ بنت حافظ عصمت اللہ صاحب</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -844,8 +882,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="6  خدیجہ  بنت دلشاد صاحب رح"&gt;6  خدیجہ  بنت دلشاد صاحب رح&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E8" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>6    خدیجہ  بنت دلشاد صاحب رح</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -857,8 +899,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="7  ذکری بنت جاوید حسین خان صاحب "&gt;7  ذکری بنت جاوید حسین خان صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E9" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">7    ذکری بنت جاوید حسین خان صاحب </v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -870,8 +916,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="8  رضا بنت نوشاد صاحب"&gt;8  رضا بنت نوشاد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E10" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>8    رضا بنت نوشاد صاحب</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -883,8 +933,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="9  زینب بنت بدرالزماں صاحب"&gt;9  زینب بنت بدرالزماں صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E11" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>9    زینب بنت بدرالزماں صاحب</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -896,8 +950,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="10  زینت خاتون بنت عبد الحسن صاحب"&gt;10  زینت خاتون بنت عبد الحسن صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E12" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>10    زینت خاتون بنت عبد الحسن صاحب</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -909,8 +967,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="11  شیزان رحمت بن رحمت علی صاحب (بستی)"&gt;11  شیزان رحمت بن رحمت علی صاحب (بستی)&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E13" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>11    شیزان رحمت بن رحمت علی صاحب (بستی)</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -922,8 +984,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="12  صفوان بن رحمت علی  صاحب (بستی)"&gt;12  صفوان بن رحمت علی  صاحب (بستی)&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E14" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>12    صفوان بن رحمت علی  صاحب (بستی)</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -935,8 +1001,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="13  عائشہ بنت  محمّد معشوق صاحب"&gt;13  عائشہ بنت  محمّد معشوق صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E15" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>13    عائشہ بنت  محمّد معشوق صاحب</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -948,8 +1018,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="14  عبدالصمد  بن محمّد شفیع صاحب"&gt;14  عبدالصمد  بن محمّد شفیع صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>14    عبدالصمد  بن محمّد شفیع صاحب</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -961,8 +1035,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="15  علیشا بنت دلشاد صاحب رح"&gt;15  علیشا بنت دلشاد صاحب رح&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>15    علیشا بنت دلشاد صاحب رح</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -974,8 +1052,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="16  عیاض احمد بن فرحت حسین صاحب"&gt;16  عیاض احمد بن فرحت حسین صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E18" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>16    عیاض احمد بن فرحت حسین صاحب</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -987,8 +1069,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="17  عیاض احمد بن وسیم احمد صاحب"&gt;17  عیاض احمد بن وسیم احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E19" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>17    عیاض احمد بن وسیم احمد صاحب</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1000,8 +1086,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="18  فضا بنت قاری صفی اللہ  صاحب"&gt;18  فضا بنت قاری صفی اللہ  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E20" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>18    فضا بنت قاری صفی اللہ  صاحب</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1013,8 +1103,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="19  فہد صادق بن عبد الصادق صاحب رح"&gt;19  فہد صادق بن عبد الصادق صاحب رح&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E21" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>19    فہد صادق بن عبد الصادق صاحب رح</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1026,8 +1120,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="20  محمّد  فہد  بن غیاث صاحب"&gt;20  محمّد  فہد  بن غیاث صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E22" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>20    محمّد  فہد  بن غیاث صاحب</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1039,8 +1137,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="21  محمّد  مصطفیٰ بن فرمان حشمت صاحب"&gt;21  محمّد  مصطفیٰ بن فرمان حشمت صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E23" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>21    محمّد  مصطفیٰ بن فرمان حشمت صاحب</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1052,8 +1154,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="22  محمّد ابان بن محمّد عامر صاحب"&gt;22  محمّد ابان بن محمّد عامر صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E24" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>22    محمّد ابان بن محمّد عامر صاحب</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1065,8 +1171,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="23  محمّد ابراہیم بن محمّد ارشاد  صاحب"&gt;23  محمّد ابراہیم بن محمّد ارشاد  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E25" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>23    محمّد ابراہیم بن محمّد ارشاد  صاحب</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1078,8 +1188,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="24  محمّد احتشام بن قاری صفی الله صاحب"&gt;24  محمّد احتشام بن قاری صفی الله صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E26" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>24    محمّد احتشام بن قاری صفی الله صاحب</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1091,8 +1205,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="25  محمّد اذلان بن علیم عارف صاحب"&gt;25  محمّد اذلان بن علیم عارف صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E27" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>25    محمّد اذلان بن علیم عارف صاحب</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1104,8 +1222,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="26  محمّد اذہان بن پرویز احمد صاحب"&gt;26  محمّد اذہان بن پرویز احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E28" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>26    محمّد اذہان بن پرویز احمد صاحب</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1117,8 +1239,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="27  محمّد ارحان بن محمّد اختر صاحب"&gt;27  محمّد ارحان بن محمّد اختر صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E29" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>27    محمّد ارحان بن محمّد اختر صاحب</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1130,8 +1256,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="28  محمّد ارحم بن   قمر الہدی صاحب"&gt;28  محمّد ارحم بن   قمر الہدی صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E30" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>28    محمّد ارحم بن   قمر الہدی صاحب</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1143,8 +1273,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="29  محمّد ارسلان بن محمّد افضل صاحب"&gt;29  محمّد ارسلان بن محمّد افضل صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E31" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>29    محمّد ارسلان بن محمّد افضل صاحب</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1156,8 +1290,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="30  محمّد ارکان بن محمّد محفوظ صاحب"&gt;30  محمّد ارکان بن محمّد محفوظ صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E32" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>30    محمّد ارکان بن محمّد محفوظ صاحب</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1169,8 +1307,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="31  محمّد الحم بن افروز اختر صاحب"&gt;31  محمّد الحم بن افروز اختر صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E33" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>31    محمّد الحم بن افروز اختر صاحب</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -1182,8 +1324,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="32  محمّد امان بن الطاف احمد صاحب"&gt;32  محمّد امان بن الطاف احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E34" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>32    محمّد امان بن الطاف احمد صاحب</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -1195,8 +1341,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="33  محمّد امان بن بدر الزماں صاحب "&gt;33  محمّد امان بن بدر الزماں صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E35" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">33    محمّد امان بن بدر الزماں صاحب </v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -1208,8 +1358,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="34  محمّد امان بن راشد الحق صاحب"&gt;34  محمّد امان بن راشد الحق صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E36" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>34    محمّد امان بن راشد الحق صاحب</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -1221,8 +1375,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="35  محمّد انس بن   محمّد چاند صاحب"&gt;35  محمّد انس بن   محمّد چاند صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E37" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>35    محمّد انس بن   محمّد چاند صاحب</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -1234,8 +1392,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="36  محمّد ایذان بن محمّد عالم صاحب"&gt;36  محمّد ایذان بن محمّد عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E38" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>36    محمّد ایذان بن محمّد عالم صاحب</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -1247,8 +1409,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="37  محمّد آشد  بن غیاث  صاحب"&gt;37  محمّد آشد  بن غیاث  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E39" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>37    محمّد آشد  بن غیاث  صاحب</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -1260,8 +1426,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="38  محمّد آفرید بن وسیم احمد صاحب "&gt;38  محمّد آفرید بن وسیم احمد صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E40" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">38    محمّد آفرید بن وسیم احمد صاحب </v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -1273,8 +1443,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="39  محمّد بلال بن انور حسین صاحب"&gt;39  محمّد بلال بن انور حسین صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E41" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>39    محمّد بلال بن انور حسین صاحب</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -1286,8 +1460,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="40  محمّد تنزیل  بن حسن مطلوب صاحب"&gt;40  محمّد تنزیل  بن حسن مطلوب صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E42" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>40    محمّد تنزیل  بن حسن مطلوب صاحب</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -1299,8 +1477,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="41  محمّد تہشیم   بن  ندیم  احمد صاحب"&gt;41  محمّد تہشیم   بن  ندیم  احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E43" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>41    محمّد تہشیم   بن  ندیم  احمد صاحب</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -1312,8 +1494,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="42  محمّد توحیدبن حسن مطلوب صاحب"&gt;42  محمّد توحیدبن حسن مطلوب صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E44" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>42    محمّد توحیدبن حسن مطلوب صاحب</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -1325,8 +1511,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="43  محمّد حمّاد بن عدیل  احمد  صاحب"&gt;43  محمّد حمّاد بن عدیل  احمد  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E45" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>43    محمّد حمّاد بن عدیل  احمد  صاحب</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -1338,8 +1528,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="44  محمّد حمزہ   اسرائیل صاحب"&gt;44  محمّد حمزہ   اسرائیل صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E46" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>44    محمّد حمزہ   اسرائیل صاحب</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -1351,8 +1545,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="45  محمّد حمزہ  بن غلام رسول صاحب "&gt;45  محمّد حمزہ  بن غلام رسول صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E47" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">45    محمّد حمزہ  بن غلام رسول صاحب </v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -1364,8 +1562,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="46  محمّد حمزہ بن مہتاب عالم صاحب"&gt;46  محمّد حمزہ بن مہتاب عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E48" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>46    محمّد حمزہ بن مہتاب عالم صاحب</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -1377,8 +1579,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="47  محمّد حمید بن شاداب عالم صاحب"&gt;47  محمّد حمید بن شاداب عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E49" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>47    محمّد حمید بن شاداب عالم صاحب</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -1390,8 +1596,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="48  محمّد حنیف بن ملک الافضل صاحب "&gt;48  محمّد حنیف بن ملک الافضل صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E50" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">48    محمّد حنیف بن ملک الافضل صاحب </v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -1403,8 +1613,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="49  محمّد دارین بن محمّد عامر صاحب"&gt;49  محمّد دارین بن محمّد عامر صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E51" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>49    محمّد دارین بن محمّد عامر صاحب</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -1416,8 +1630,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="50  محمّد دانش بن نصیر احمد صاحب"&gt;50  محمّد دانش بن نصیر احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E52" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>50    محمّد دانش بن نصیر احمد صاحب</v>
+      </c>
+    </row>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53">
         <f t="shared" si="0"/>
         <v>51</v>
@@ -1429,8 +1647,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="51  محمّد داؤد بن خواجہ فرید الدین  صاحب"&gt;51  محمّد داؤد بن خواجہ فرید الدین  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E53" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>51    محمّد داؤد بن خواجہ فرید الدین  صاحب</v>
+      </c>
+    </row>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54">
         <f t="shared" si="0"/>
         <v>52</v>
@@ -1442,8 +1664,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="52  محمّد راشد بن رازق حسین خان صاحب"&gt;52  محمّد راشد بن رازق حسین خان صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E54" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>52    محمّد راشد بن رازق حسین خان صاحب</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55">
         <f t="shared" si="0"/>
         <v>53</v>
@@ -1455,8 +1681,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="53  محمّد ریحان  بن شمیم عالم صاحب"&gt;53  محمّد ریحان  بن شمیم عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E55" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>53    محمّد ریحان  بن شمیم عالم صاحب</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56">
         <f t="shared" si="0"/>
         <v>54</v>
@@ -1468,8 +1698,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="54  محمّد ریحان بن اظہار احمد صاحب"&gt;54  محمّد ریحان بن اظہار احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E56" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>54    محمّد ریحان بن اظہار احمد صاحب</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57">
         <f t="shared" si="0"/>
         <v>55</v>
@@ -1481,8 +1715,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="55  محمّد زیان بن رضوان خان صاحب"&gt;55  محمّد زیان بن رضوان خان صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E57" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>55    محمّد زیان بن رضوان خان صاحب</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58">
         <f t="shared" si="0"/>
         <v>56</v>
@@ -1494,8 +1732,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="56  محمّد زید بن  افتخار  احمد  صاحب"&gt;56  محمّد زید بن  افتخار  احمد  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E58" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>56    محمّد زید بن  افتخار  احمد  صاحب</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59">
         <f t="shared" si="0"/>
         <v>57</v>
@@ -1507,8 +1749,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="57  محمّد زید بن حافظ فیض الرحمن صاحب"&gt;57  محمّد زید بن حافظ فیض الرحمن صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E59" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>57    محمّد زید بن حافظ فیض الرحمن صاحب</v>
+      </c>
+    </row>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60">
         <f t="shared" si="0"/>
         <v>58</v>
@@ -1520,8 +1766,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="58  محمّد زید بن ظہیر الدین صاحب"&gt;58  محمّد زید بن ظہیر الدین صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E60" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>58    محمّد زید بن ظہیر الدین صاحب</v>
+      </c>
+    </row>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61">
         <f t="shared" si="0"/>
         <v>59</v>
@@ -1533,8 +1783,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="59  محمّد سفیان بن شفقت الله صاحب"&gt;59  محمّد سفیان بن شفقت الله صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E61" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>59    محمّد سفیان بن شفقت الله صاحب</v>
+      </c>
+    </row>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62">
         <f t="shared" si="0"/>
         <v>60</v>
@@ -1546,8 +1800,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="60  محمّد شادمان  بن محمّد ارشاد صاحب"&gt;60  محمّد شادمان  بن محمّد ارشاد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E62" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>60    محمّد شادمان  بن محمّد ارشاد صاحب</v>
+      </c>
+    </row>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63">
         <f t="shared" si="0"/>
         <v>61</v>
@@ -1559,8 +1817,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="61  محمّد شمس بن پرویز لاری صاحب"&gt;61  محمّد شمس بن پرویز لاری صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E63" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>61    محمّد شمس بن پرویز لاری صاحب</v>
+      </c>
+    </row>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64">
         <f t="shared" si="0"/>
         <v>62</v>
@@ -1572,8 +1834,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="62  محمّد صالق بن واثق باللہ صاحب"&gt;62  محمّد صالق بن واثق باللہ صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E64" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>62    محمّد صالق بن واثق باللہ صاحب</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65">
         <f t="shared" si="0"/>
         <v>63</v>
@@ -1585,8 +1851,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="63  محمّد صائم بن محمّد فیصل صاحب"&gt;63  محمّد صائم بن محمّد فیصل صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E65" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>63    محمّد صائم بن محمّد فیصل صاحب</v>
+      </c>
+    </row>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66">
         <f t="shared" si="0"/>
         <v>64</v>
@@ -1598,8 +1868,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="64  محمّد صفوان بن محمّد قیصر عالم صاحب"&gt;64  محمّد صفوان بن محمّد قیصر عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E66" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>64    محمّد صفوان بن محمّد قیصر عالم صاحب</v>
+      </c>
+    </row>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67">
         <f t="shared" ref="B67:B97" si="1">IF(C67="","",ROW(A65))</f>
         <v>65</v>
@@ -1611,8 +1885,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="65  محمّد طیّب  بن مہتاب عالم صاحب"&gt;65  محمّد طیّب  بن مہتاب عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E67" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>65    محمّد طیّب  بن مہتاب عالم صاحب</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68">
         <f t="shared" si="1"/>
         <v>66</v>
@@ -1624,8 +1902,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="66  محمّد عابدبن حافظ عمران صاحب"&gt;66  محمّد عابدبن حافظ عمران صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E68" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>66    محمّد عابدبن حافظ عمران صاحب</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69">
         <f t="shared" si="1"/>
         <v>67</v>
@@ -1637,8 +1919,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="67  محمّد عارش  بن علیم الدین صاحب"&gt;67  محمّد عارش  بن علیم الدین صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E69" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>67    محمّد عارش  بن علیم الدین صاحب</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70">
         <f t="shared" si="1"/>
         <v>68</v>
@@ -1650,8 +1936,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="68  محمّد عاکف بن قمرالہدی صاحب"&gt;68  محمّد عاکف بن قمرالہدی صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E70" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>68    محمّد عاکف بن قمرالہدی صاحب</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71">
         <f t="shared" si="1"/>
         <v>69</v>
@@ -1663,8 +1953,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="69  محمّد عاہل بن محمّد دانش  صاحب"&gt;69  محمّد عاہل بن محمّد دانش  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E71" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>69    محمّد عاہل بن محمّد دانش  صاحب</v>
+      </c>
+    </row>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72">
         <f t="shared" si="1"/>
         <v>70</v>
@@ -1676,8 +1970,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="70  محمّد عدنان بن محمّد افضل صاحب"&gt;70  محمّد عدنان بن محمّد افضل صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E72" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>70    محمّد عدنان بن محمّد افضل صاحب</v>
+      </c>
+    </row>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B73">
         <f t="shared" si="1"/>
         <v>71</v>
@@ -1689,8 +1987,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="71  محمّد عزیر بن ممتاز احمد صاحب"&gt;71  محمّد عزیر بن ممتاز احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E73" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>71    محمّد عزیر بن ممتاز احمد صاحب</v>
+      </c>
+    </row>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B74">
         <f t="shared" si="1"/>
         <v>72</v>
@@ -1702,8 +2004,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="72  محمّد علی بن نوید احمد صاحب"&gt;72  محمّد علی بن نوید احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E74" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>72    محمّد علی بن نوید احمد صاحب</v>
+      </c>
+    </row>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B75">
         <f t="shared" si="1"/>
         <v>73</v>
@@ -1715,8 +2021,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="73  محمّد عمر بن عبد الرزاق صاحب"&gt;73  محمّد عمر بن عبد الرزاق صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E75" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>73    محمّد عمر بن عبد الرزاق صاحب</v>
+      </c>
+    </row>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B76">
         <f t="shared" si="1"/>
         <v>74</v>
@@ -1728,8 +2038,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="74  محمّد عمر بن گلریز احمد خان صاحب"&gt;74  محمّد عمر بن گلریز احمد خان صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E76" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>74    محمّد عمر بن گلریز احمد خان صاحب</v>
+      </c>
+    </row>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B77">
         <f t="shared" si="1"/>
         <v>75</v>
@@ -1741,8 +2055,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="75  محمّد عمیر بن نذیر الدین صاحب"&gt;75  محمّد عمیر بن نذیر الدین صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E77" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>75    محمّد عمیر بن نذیر الدین صاحب</v>
+      </c>
+    </row>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B78">
         <f t="shared" si="1"/>
         <v>76</v>
@@ -1754,8 +2072,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="76  محمّد عیاں بن شفیق صاحب رحمه اللہ"&gt;76  محمّد عیاں بن شفیق صاحب رحمه اللہ&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="79" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E78" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>76    محمّد عیاں بن شفیق صاحب رحمه اللہ</v>
+      </c>
+    </row>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B79">
         <f t="shared" si="1"/>
         <v>77</v>
@@ -1767,8 +2089,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="77  محمّد عیان بن ظہیر الدین صاحب"&gt;77  محمّد عیان بن ظہیر الدین صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="80" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E79" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>77    محمّد عیان بن ظہیر الدین صاحب</v>
+      </c>
+    </row>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B80">
         <f t="shared" si="1"/>
         <v>78</v>
@@ -1780,8 +2106,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="78  محمّد فرحان بن شمیم عالم صاحب"&gt;78  محمّد فرحان بن شمیم عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E80" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>78    محمّد فرحان بن شمیم عالم صاحب</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B81">
         <f t="shared" si="1"/>
         <v>79</v>
@@ -1793,8 +2123,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="79  محمّد فردین بن محمّد شاہد صاحب"&gt;79  محمّد فردین بن محمّد شاہد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E81" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>79    محمّد فردین بن محمّد شاہد صاحب</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B82">
         <f t="shared" si="1"/>
         <v>80</v>
@@ -1806,8 +2140,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="80  محمّد کیفی بن محمّد نواز شیروانی صاحب"&gt;80  محمّد کیفی بن محمّد نواز شیروانی صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E82" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>80    محمّد کیفی بن محمّد نواز شیروانی صاحب</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B83">
         <f t="shared" si="1"/>
         <v>81</v>
@@ -1819,8 +2157,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="81  محمّد محتشم بن محمّد عامر صاحب"&gt;81  محمّد محتشم بن محمّد عامر صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E83" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>81    محمّد محتشم بن محمّد عامر صاحب</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B84">
         <f t="shared" si="1"/>
         <v>82</v>
@@ -1832,8 +2174,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="82  محمّد مدّثر بن شکیل احمد  صاحب"&gt;82  محمّد مدّثر بن شکیل احمد  صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E84" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>82    محمّد مدّثر بن شکیل احمد  صاحب</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B85">
         <f t="shared" si="1"/>
         <v>83</v>
@@ -1845,8 +2191,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="83  محمّد مزمل بن شکیل احمد صاحب"&gt;83  محمّد مزمل بن شکیل احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E85" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>83    محمّد مزمل بن شکیل احمد صاحب</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B86">
         <f t="shared" si="1"/>
         <v>84</v>
@@ -1858,8 +2208,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="84  محمّد معروف بن  محمّد معشوق صاحب"&gt;84  محمّد معروف بن  محمّد معشوق صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E86" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>84    محمّد معروف بن  محمّد معشوق صاحب</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B87">
         <f t="shared" si="1"/>
         <v>85</v>
@@ -1871,8 +2225,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="85  محمّد ہادی بن ملک العزیز صاحب"&gt;85  محمّد ہادی بن ملک العزیز صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E87" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>85    محمّد ہادی بن ملک العزیز صاحب</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B88">
         <f t="shared" si="1"/>
         <v>86</v>
@@ -1884,8 +2242,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="86  محمّد ھود "&gt;86  محمّد ھود &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E88" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">86    محمّد ھود </v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B89">
         <f t="shared" si="1"/>
         <v>87</v>
@@ -1897,8 +2259,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="87  محمّد یوسف بن ذرار صاحب"&gt;87  محمّد یوسف بن ذرار صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E89" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>87    محمّد یوسف بن ذرار صاحب</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B90">
         <f t="shared" si="1"/>
         <v>88</v>
@@ -1910,8 +2276,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="88  محمّد یوسف بن محمّد بلال صاحب "&gt;88  محمّد یوسف بن محمّد بلال صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E90" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">88    محمّد یوسف بن محمّد بلال صاحب </v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B91">
         <f t="shared" si="1"/>
         <v>89</v>
@@ -1923,8 +2293,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="89  محمّداحتشام بن نعیم خان صاحب"&gt;89  محمّداحتشام بن نعیم خان صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E91" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>89    محمّداحتشام بن نعیم خان صاحب</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B92">
         <f t="shared" si="1"/>
         <v>90</v>
@@ -1936,8 +2310,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="90  محمّدشدیب  بن محمّد عالم صاحب"&gt;90  محمّدشدیب  بن محمّد عالم صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E92" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>90    محمّدشدیب  بن محمّد عالم صاحب</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B93">
         <f t="shared" si="1"/>
         <v>91</v>
@@ -1949,8 +2327,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="91  محمّدعرش  بن عبد الرحیم صاحب "&gt;91  محمّدعرش  بن عبد الرحیم صاحب &lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E93" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v xml:space="preserve">91    محمّدعرش  بن عبد الرحیم صاحب </v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B94">
         <f t="shared" si="1"/>
         <v>92</v>
@@ -1962,8 +2344,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="92  معاذ حبیب بن حبیب الله صاحب"&gt;92  معاذ حبیب بن حبیب الله صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E94" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>92    معاذ حبیب بن حبیب الله صاحب</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B95">
         <f t="shared" si="1"/>
         <v>93</v>
@@ -1975,8 +2361,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="93  معاذ رحمن بن معین الرحمن صاحب"&gt;93  معاذ رحمن بن معین الرحمن صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E95" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>93    معاذ رحمن بن معین الرحمن صاحب</v>
+      </c>
+    </row>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B96">
         <f t="shared" si="1"/>
         <v>94</v>
@@ -1988,8 +2378,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="94  وصی احمد بن رئیس احمد صاحب"&gt;94  وصی احمد بن رئیس احمد صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E96" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>94    وصی احمد بن رئیس احمد صاحب</v>
+      </c>
+    </row>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B97">
         <f t="shared" si="1"/>
         <v>95</v>
@@ -2001,8 +2395,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="95  یٰسین کاظمی بن قطب الدین  کاظمی صاحب"&gt;95  یٰسین کاظمی بن قطب الدین  کاظمی صاحب&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E97" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>95    یٰسین کاظمی بن قطب الدین  کاظمی صاحب</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B98">
         <f>IF(C98="","",ROW(A96))</f>
         <v>96</v>
@@ -2014,8 +2412,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="96  محمّد طالب بن"&gt;96  محمّد طالب بن&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E98" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>96    محمّد طالب بن</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B99">
         <f>IF(C99="","",ROW(A97))</f>
         <v>97</v>
@@ -2027,8 +2429,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="97  محمّد ذہیب بن"&gt;97  محمّد ذہیب بن&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E99" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>97    محمّد ذہیب بن</v>
+      </c>
+    </row>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B100">
         <f>IF(C100="","",ROW(A98))</f>
         <v>98</v>
@@ -2040,8 +2446,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="98  محمّد عمر بن محمّد اجمل صاحب  (مئو)"&gt;98  محمّد عمر بن محمّد اجمل صاحب  (مئو)&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E100" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>98    محمّد عمر بن محمّد اجمل صاحب  (مئو)</v>
+      </c>
+    </row>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B101">
         <f>IF(C101="","",ROW(A99))</f>
         <v>99</v>
@@ -2053,8 +2463,12 @@
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="99  محمّد زیاں بن محمّد انور صاحب (امریکا)"&gt;99  محمّد زیاں بن محمّد انور صاحب (امریکا)&lt;/option&gt;</v>
       </c>
-    </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E101" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>99    محمّد زیاں بن محمّد انور صاحب (امریکا)</v>
+      </c>
+    </row>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B102">
         <f>IF(C102="","",ROW(A100))</f>
         <v>100</v>
@@ -2065,6 +2479,10 @@
       <c r="D102" t="str">
         <f>_xlfn.CONCAT("&lt;option value=""",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"""&gt;",Table1[[#This Row],[roll-no]],"  ",Table1[[#This Row],[name]],"&lt;/option&gt;")</f>
         <v>&lt;option value="100  محمّد ریاض صاحب (جدّہ)"&gt;100  محمّد ریاض صاحب (جدّہ)&lt;/option&gt;</v>
+      </c>
+      <c r="E102" t="str">
+        <f>_xlfn.CONCAT(Table1[[#This Row],[roll-no]],"    ",Table1[[#This Row],[name]])</f>
+        <v>100    محمّد ریاض صاحب (جدّہ)</v>
       </c>
     </row>
   </sheetData>

</xml_diff>